<commit_message>
Fixed referencing mistake in Results tab
</commit_message>
<xml_diff>
--- a/Biodiversity tool_simple_v1.1.xlsx
+++ b/Biodiversity tool_simple_v1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJ35FA\Documents\Doughnut for Urban Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KJ35FA\Documents\GitHub\doughnut-biotool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F32B8F5-529D-417E-A4E8-57562EDCDE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94784C11-BD38-473F-89B7-D8FBEF97F4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-17775" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -2146,7 +2146,7 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2294,10 +2294,7 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2306,6 +2303,76 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="52">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Barlow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Barlow"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Barlow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Barlow"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2332,24 +2399,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Barlow"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0E+00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
@@ -2624,54 +2673,7 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Barlow"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="164" formatCode="0.0E+00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0E+00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Barlow"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2745,54 +2747,7 @@
         <name val="Barlow"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Barlow"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="164" formatCode="0.0E+00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Barlow"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2861,6 +2816,24 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Barlow"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0E+00"/>
     </dxf>
     <dxf>
       <font>
@@ -11917,54 +11890,56 @@
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E64F8681-32A3-4593-8DEA-5DED266A411E}" name="Product name" totalsRowLabel="Total" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{8DC48DF5-45A8-4772-950F-F437FCEB1F4D}" name="Impact (species.year)" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="3">
+    <tableColumn id="2" xr3:uid="{8DC48DF5-45A8-4772-950F-F437FCEB1F4D}" name="Impact (species.year)" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39">
       <calculatedColumnFormula>IF(VLOOKUP(Table47[[#This Row],[Product name]],Table4[],3,FALSE)=VLOOKUP(Table47[[#This Row],[Product name]],Table4[],4,FALSE),VLOOKUP(Table47[[#This Row],[Product name]],Table4[],2,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],5,FALSE),IF(VLOOKUP(Table47[[#This Row],[Product name]],Table4[],3,FALSE)="kg",VLOOKUP(Table47[[#This Row],[Product name]],Table4[],2,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],5,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],4,FALSE),IF(VLOOKUP(Table47[[#This Row],[Product name]],Table4[],3,FALSE)="m3",VLOOKUP(Table47[[#This Row],[Product name]],Table4[],2,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],5,FALSE)/VLOOKUP(Table47[[#This Row],[Product name]],Table1[],4,FALSE),"Unit error!")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{44F1C6D6-111D-4738-B833-8E40A51C9BC5}" name="Material type" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{44F1C6D6-111D-4738-B833-8E40A51C9BC5}" name="Material type" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{46F1981E-2B5E-4185-B066-997BC0914EC6}" name="Table8" displayName="Table8" ref="C8:D19" totalsRowCount="1" headerRowDxfId="38" dataDxfId="37" totalsRowDxfId="35" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{46F1981E-2B5E-4185-B066-997BC0914EC6}" name="Table8" displayName="Table8" ref="C8:D19" totalsRowCount="1" headerRowDxfId="37" dataDxfId="36" totalsRowDxfId="34" tableBorderDxfId="35">
   <autoFilter ref="C8:D18" xr:uid="{46F1981E-2B5E-4185-B066-997BC0914EC6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1F303639-3406-463D-867F-DE4D4D31EAC5}" name="Land use type" totalsRowLabel="Total" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{E9DD1703-E948-4AFA-9D58-BB22E7B8DAFE}" name="Impact (species.year)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{1F303639-3406-463D-867F-DE4D4D31EAC5}" name="Land use type" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E9DD1703-E948-4AFA-9D58-BB22E7B8DAFE}" name="Impact (species.year)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="0">
+      <calculatedColumnFormula>(Input!E21-Input!J21)*Data_land!D11+(Input!J21-Input!E21)*Input!$E$14*Data_land!D25</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{18004D57-1468-4568-AC5D-EF24B2E32C6A}" name="Table9" displayName="Table9" ref="J24:K28" totalsRowCount="1" headerRowDxfId="30" dataDxfId="29" totalsRowDxfId="27" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{18004D57-1468-4568-AC5D-EF24B2E32C6A}" name="Table9" displayName="Table9" ref="J24:K28" totalsRowCount="1" headerRowDxfId="31" dataDxfId="30" totalsRowDxfId="28" tableBorderDxfId="29">
   <autoFilter ref="J24:K27" xr:uid="{18004D57-1468-4568-AC5D-EF24B2E32C6A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B3ADFC0E-1A5C-473D-AD3D-438698B4A20E}" name="Energy use" totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{384AB5A9-CE6A-470F-A2F8-DD2BCC603078}" name="Impact (species.year)" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{B3ADFC0E-1A5C-473D-AD3D-438698B4A20E}" name="Energy use" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{384AB5A9-CE6A-470F-A2F8-DD2BCC603078}" name="Impact (species.year)" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{B57E9357-9C44-4FB1-BD81-C3BAFF347ADC}" name="Table10" displayName="Table10" ref="J33:K36" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{B57E9357-9C44-4FB1-BD81-C3BAFF347ADC}" name="Table10" displayName="Table10" ref="J33:K36" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="J33:K36" xr:uid="{B57E9357-9C44-4FB1-BD81-C3BAFF347ADC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B783EF1E-20B6-4D0B-A433-3FAF65E7E52B}" name="Source of biodiversity impacts" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{676C2152-473E-4D1E-AD54-3B76DDAFE759}" name="Impact (species.year)" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{B783EF1E-20B6-4D0B-A433-3FAF65E7E52B}" name="Source of biodiversity impacts" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{676C2152-473E-4D1E-AD54-3B76DDAFE759}" name="Impact (species.year)" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7B6839B2-3F41-4A52-9B2F-D040812516DC}" name="Table11" displayName="Table11" ref="C94:D110" totalsRowCount="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7B6839B2-3F41-4A52-9B2F-D040812516DC}" name="Table11" displayName="Table11" ref="C94:D110" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="19">
   <autoFilter ref="C94:D109" xr:uid="{7B6839B2-3F41-4A52-9B2F-D040812516DC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3BA63C1E-2355-46B2-807B-F572240361CC}" name="Material type" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{358697AB-1B8D-4930-A116-11FC8431B0E6}" name="Total biodiversity impact (species.year)" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="1" xr3:uid="{3BA63C1E-2355-46B2-807B-F572240361CC}" name="Material type" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{358697AB-1B8D-4930-A116-11FC8431B0E6}" name="Total biodiversity impact (species.year)" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula>SUMIF(Table47[Material type],C95,Table47[Impact (species.year)])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -11973,18 +11948,18 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DC07F33-EE7A-41E9-9601-56B623D8C715}" name="Table3" displayName="Table3" ref="A7:F108" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DC07F33-EE7A-41E9-9601-56B623D8C715}" name="Table3" displayName="Table3" ref="A7:F108" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <autoFilter ref="A7:F108" xr:uid="{4DC07F33-EE7A-41E9-9601-56B623D8C715}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:F108">
     <sortCondition ref="A7:A108"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{87FAC7EB-2713-436E-9742-0B29EE7AFC3B}" name="Ecoinvent process (v3.9.1)" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="7" xr3:uid="{384622DF-FAF1-44E9-9FF1-5153F2AE15DF}" name="Geography" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{D8F4E4C3-5A1E-4D87-888A-90D9AEAB7B74}" name="Product name" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{6EDC8070-85B9-4DEC-A29D-F47B5412B2C3}" name="Ecoinvent unit" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{99ED5211-1C19-4C05-ADFE-7101B564E1F5}" name="Density (kg/m3)" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{E96CD1D0-BAB7-4F1E-86EE-0574E4DAF2E2}" name="Biodiversity impact (species.year per unit)" dataDxfId="4" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{87FAC7EB-2713-436E-9742-0B29EE7AFC3B}" name="Ecoinvent process (v3.9.1)" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{384622DF-FAF1-44E9-9FF1-5153F2AE15DF}" name="Geography" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{D8F4E4C3-5A1E-4D87-888A-90D9AEAB7B74}" name="Product name" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{6EDC8070-85B9-4DEC-A29D-F47B5412B2C3}" name="Ecoinvent unit" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{99ED5211-1C19-4C05-ADFE-7101B564E1F5}" name="Density (kg/m3)" dataDxfId="8" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{E96CD1D0-BAB7-4F1E-86EE-0574E4DAF2E2}" name="Biodiversity impact (species.year per unit)" dataDxfId="7" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -12644,8 +12619,8 @@
   </sheetPr>
   <dimension ref="B1:AE261"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA77" sqref="AA77"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -14215,13 +14190,13 @@
         <v>458</v>
       </c>
       <c r="Q47" s="45"/>
-      <c r="R47" s="120" t="s">
+      <c r="R47" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="S47" s="120" t="s">
+      <c r="S47" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="T47" s="120" t="s">
+      <c r="T47" s="20" t="s">
         <v>154</v>
       </c>
       <c r="U47" s="56"/>
@@ -14386,14 +14361,14 @@
       <c r="M54" s="15"/>
       <c r="N54" s="56"/>
       <c r="O54" s="48"/>
-      <c r="P54" s="120" t="s">
+      <c r="P54" s="20" t="s">
         <v>462</v>
       </c>
       <c r="Q54" s="45"/>
-      <c r="R54" s="120" t="s">
+      <c r="R54" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="S54" s="120" t="s">
+      <c r="S54" s="20" t="s">
         <v>38</v>
       </c>
       <c r="T54" s="20" t="s">
@@ -15231,13 +15206,13 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="J31">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>$E$31</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>$E$32</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>$E$32</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15269,8 +15244,8 @@
   </sheetPr>
   <dimension ref="A2:O111"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -15342,7 +15317,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="30">
-        <f>(Input!E21-Input!J21)*Data_land!D11+(Input!J21-Input!E21)*Input!$Y$18*Data_land!D25</f>
+        <f>(Input!E21-Input!J21)*Data_land!D11+(Input!J21-Input!E21)*Input!$E$14*Data_land!D25</f>
         <v>0</v>
       </c>
       <c r="E9" s="32"/>
@@ -15354,7 +15329,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="30">
-        <f>(Input!E22-Input!J22)*Data_land!D12+(Input!J22-Input!E22)*Input!$Y$18*Data_land!D26</f>
+        <f>(Input!E22-Input!J22)*Data_land!D12+(Input!J22-Input!E22)*Input!$E$14*Data_land!D26</f>
         <v>0</v>
       </c>
       <c r="E10" s="32"/>
@@ -15366,7 +15341,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="30">
-        <f>(Input!E23-Input!J23)*Data_land!D13+(Input!J23-Input!E23)*Input!$Y$18*Data_land!D27</f>
+        <f>(Input!E23-Input!J23)*Data_land!D13+(Input!J23-Input!E23)*Input!$E$14*Data_land!D27</f>
         <v>0</v>
       </c>
       <c r="E11" s="32"/>
@@ -15378,7 +15353,7 @@
         <v>28</v>
       </c>
       <c r="D12" s="30">
-        <f>(Input!E24-Input!J24)*Data_land!D14+(Input!J24-Input!E24)*Input!$Y$18*Data_land!D28</f>
+        <f>(Input!E24-Input!J24)*Data_land!D14+(Input!J24-Input!E24)*Input!$E$14*Data_land!D28</f>
         <v>0</v>
       </c>
       <c r="E12" s="32"/>
@@ -15390,7 +15365,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="30">
-        <f>(Input!E25-Input!J25)*Data_land!D15+(Input!J25-Input!E25)*Input!$Y$18*Data_land!D29</f>
+        <f>(Input!E25-Input!J25)*Data_land!D15+(Input!J25-Input!E25)*Input!$E$14*Data_land!D29</f>
         <v>0</v>
       </c>
       <c r="E13" s="32"/>
@@ -15402,7 +15377,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="30">
-        <f>(Input!E26-Input!J26)*Data_land!D16+(Input!J26-Input!E26)*Input!$Y$18*Data_land!D30</f>
+        <f>(Input!E26-Input!J26)*Data_land!D16+(Input!J26-Input!E26)*Input!$E$14*Data_land!D30</f>
         <v>0</v>
       </c>
       <c r="E14" s="32"/>
@@ -15414,7 +15389,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="30">
-        <f>(Input!E27-Input!J27)*Data_land!D17+(Input!J27-Input!E27)*Input!$Y$18*Data_land!D31</f>
+        <f>(Input!E27-Input!J27)*Data_land!D17+(Input!J27-Input!E27)*Input!$E$14*Data_land!D31</f>
         <v>0</v>
       </c>
       <c r="E15" s="32"/>
@@ -15426,7 +15401,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="30">
-        <f>(Input!E28-Input!J28)*Data_land!D18+(Input!J28-Input!E28)*Input!$Y$18*Data_land!D32</f>
+        <f>(Input!E28-Input!J28)*Data_land!D18+(Input!J28-Input!E28)*Input!$E$14*Data_land!D32</f>
         <v>0</v>
       </c>
       <c r="E16" s="32"/>
@@ -15438,7 +15413,7 @@
         <v>34</v>
       </c>
       <c r="D17" s="30">
-        <f>(Input!E29-Input!J29)*Data_land!D19+(Input!J29-Input!E29)*Input!$Y$18*Data_land!D33</f>
+        <f>(Input!E29-Input!J29)*Data_land!D19+(Input!J29-Input!E29)*Input!$E$14*Data_land!D33</f>
         <v>0</v>
       </c>
       <c r="E17" s="32"/>
@@ -15450,7 +15425,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="30">
-        <f>(Input!E30-Input!J30)*Data_land!D20+(Input!J30-Input!E30)*Input!$Y$18*Data_land!D34</f>
+        <f>(Input!E30-Input!J30)*Data_land!D20+(Input!J30-Input!E30)*Input!$E$14*Data_land!D34</f>
         <v>0</v>
       </c>
       <c r="E18" s="32"/>
@@ -15598,7 +15573,7 @@
         <v>362</v>
       </c>
       <c r="K27" s="30">
-        <f>-Input!Y17*VLOOKUP(Results!J25,Table1[],5,FALSE)*Input!E$16</f>
+        <f>-Input!Y19*VLOOKUP(Results!J25,Table1[],5,FALSE)*Input!E$14</f>
         <v>0</v>
       </c>
       <c r="L27" s="80"/>
@@ -16229,10 +16204,10 @@
     <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="12"/>
       <c r="B64" s="48"/>
-      <c r="C64" s="117" t="s">
+      <c r="C64" t="s">
         <v>462</v>
       </c>
-      <c r="D64" s="119">
+      <c r="D64" s="30">
         <f>IF(VLOOKUP(Table47[[#This Row],[Product name]],Table4[],3,FALSE)=VLOOKUP(Table47[[#This Row],[Product name]],Table4[],4,FALSE),VLOOKUP(Table47[[#This Row],[Product name]],Table4[],2,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],5,FALSE),IF(VLOOKUP(Table47[[#This Row],[Product name]],Table4[],3,FALSE)="kg",VLOOKUP(Table47[[#This Row],[Product name]],Table4[],2,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],5,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],4,FALSE),IF(VLOOKUP(Table47[[#This Row],[Product name]],Table4[],3,FALSE)="m3",VLOOKUP(Table47[[#This Row],[Product name]],Table4[],2,FALSE)*VLOOKUP(Table47[[#This Row],[Product name]],Table1[],5,FALSE)/VLOOKUP(Table47[[#This Row],[Product name]],Table1[],4,FALSE),"Unit error!")))</f>
         <v>0</v>
       </c>
@@ -18641,7 +18616,7 @@
   <dimension ref="B2:R58"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -19111,7 +19086,7 @@
       <c r="E8">
         <v>1200</v>
       </c>
-      <c r="F8" s="118">
+      <c r="F8" s="117">
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J8" t="s">
@@ -19150,7 +19125,7 @@
       <c r="E9">
         <v>2700</v>
       </c>
-      <c r="F9" s="118">
+      <c r="F9" s="117">
         <v>2.4999999999999999E-8</v>
       </c>
       <c r="J9" t="s">
@@ -19186,7 +19161,7 @@
       <c r="E10">
         <v>2970</v>
       </c>
-      <c r="F10" s="118">
+      <c r="F10" s="117">
         <v>5.0000000000000003E-10</v>
       </c>
       <c r="J10" t="s">
@@ -19222,7 +19197,7 @@
       <c r="E11">
         <v>2300</v>
       </c>
-      <c r="F11" s="118">
+      <c r="F11" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J11" t="s">
@@ -19261,7 +19236,7 @@
       <c r="E12">
         <v>7850</v>
       </c>
-      <c r="F12" s="118">
+      <c r="F12" s="117">
         <v>7.4999999999999993E-9</v>
       </c>
       <c r="J12" t="s">
@@ -19297,7 +19272,7 @@
       <c r="E13">
         <v>65</v>
       </c>
-      <c r="F13" s="118">
+      <c r="F13" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J13" t="s">
@@ -19333,7 +19308,7 @@
       <c r="E14">
         <v>2300</v>
       </c>
-      <c r="F14" s="118">
+      <c r="F14" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J14" t="s">
@@ -19369,7 +19344,7 @@
       <c r="E15">
         <v>2160</v>
       </c>
-      <c r="F15" s="118">
+      <c r="F15" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J15" t="s">
@@ -19405,7 +19380,7 @@
       <c r="E16">
         <v>2160</v>
       </c>
-      <c r="F16" s="118">
+      <c r="F16" s="117">
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="J16" t="s">
@@ -19441,7 +19416,7 @@
       <c r="E17">
         <v>2600</v>
       </c>
-      <c r="F17" s="118">
+      <c r="F17" s="117">
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="J17" t="s">
@@ -19477,7 +19452,7 @@
       <c r="E18">
         <v>1700</v>
       </c>
-      <c r="F18" s="118">
+      <c r="F18" s="117">
         <v>5.0000000000000002E-11</v>
       </c>
       <c r="J18" t="s">
@@ -19516,7 +19491,7 @@
       <c r="E19">
         <v>1920</v>
       </c>
-      <c r="F19" s="118">
+      <c r="F19" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J19" t="s">
@@ -19555,7 +19530,7 @@
       <c r="E20">
         <v>2300</v>
       </c>
-      <c r="F20" s="118">
+      <c r="F20" s="117">
         <v>5.0000000000000003E-10</v>
       </c>
       <c r="J20" t="s">
@@ -19591,7 +19566,7 @@
       <c r="E21">
         <v>2200</v>
       </c>
-      <c r="F21" s="118">
+      <c r="F21" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J21" t="s">
@@ -19627,7 +19602,7 @@
       <c r="E22">
         <v>2200</v>
       </c>
-      <c r="F22" s="118">
+      <c r="F22" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J22" t="s">
@@ -19663,7 +19638,7 @@
       <c r="E23">
         <v>2200</v>
       </c>
-      <c r="F23" s="118">
+      <c r="F23" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J23" t="s">
@@ -19702,7 +19677,7 @@
       <c r="E24">
         <v>2200</v>
       </c>
-      <c r="F24" s="118">
+      <c r="F24" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J24" t="s">
@@ -19741,7 +19716,7 @@
       <c r="E25">
         <v>2200</v>
       </c>
-      <c r="F25" s="118">
+      <c r="F25" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J25" t="s">
@@ -19780,7 +19755,7 @@
       <c r="E26">
         <v>2200</v>
       </c>
-      <c r="F26" s="118">
+      <c r="F26" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J26" t="s">
@@ -19816,7 +19791,7 @@
       <c r="E27">
         <v>2300</v>
       </c>
-      <c r="F27" s="118">
+      <c r="F27" s="117">
         <v>7.5E-10</v>
       </c>
       <c r="J27" t="s">
@@ -19852,7 +19827,7 @@
       <c r="E28">
         <v>2300</v>
       </c>
-      <c r="F28" s="118">
+      <c r="F28" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J28" t="s">
@@ -19888,7 +19863,7 @@
       <c r="E29">
         <v>490</v>
       </c>
-      <c r="F29" s="118">
+      <c r="F29" s="117">
         <v>7.5000000000000002E-6</v>
       </c>
       <c r="J29" t="s">
@@ -19921,7 +19896,7 @@
       <c r="D30" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="118">
+      <c r="F30" s="117">
         <v>7.5000000000000002E-7</v>
       </c>
       <c r="J30" t="s">
@@ -19954,7 +19929,7 @@
       <c r="D31" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="118">
+      <c r="F31" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J31" t="s">
@@ -19990,7 +19965,7 @@
       <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="118">
+      <c r="F32" s="117">
         <v>7.5000000000000002E-7</v>
       </c>
       <c r="J32" t="s">
@@ -20026,7 +20001,7 @@
       <c r="E33">
         <v>1580</v>
       </c>
-      <c r="F33" s="118">
+      <c r="F33" s="117">
         <v>7.4999999999999993E-9</v>
       </c>
       <c r="J33" t="s">
@@ -20065,7 +20040,7 @@
       <c r="E34">
         <v>1580</v>
       </c>
-      <c r="F34" s="118">
+      <c r="F34" s="117">
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="J34" t="s">
@@ -20101,7 +20076,7 @@
       <c r="E35">
         <v>900</v>
       </c>
-      <c r="F35" s="118">
+      <c r="F35" s="117">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J35" t="s">
@@ -20134,7 +20109,7 @@
       <c r="E36">
         <v>700</v>
       </c>
-      <c r="F36" s="118">
+      <c r="F36" s="117">
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="J36" t="s">
@@ -20167,7 +20142,7 @@
       <c r="E37">
         <v>1300</v>
       </c>
-      <c r="F37" s="118">
+      <c r="F37" s="117">
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="J37" t="s">
@@ -20200,7 +20175,7 @@
       <c r="E38">
         <v>20</v>
       </c>
-      <c r="F38" s="118">
+      <c r="F38" s="117">
         <v>1E-8</v>
       </c>
       <c r="J38" t="s">
@@ -20233,7 +20208,7 @@
       <c r="E39">
         <v>20</v>
       </c>
-      <c r="F39" s="118">
+      <c r="F39" s="117">
         <v>2.4999999999999999E-7</v>
       </c>
       <c r="J39" t="s">
@@ -20269,7 +20244,7 @@
       <c r="E40">
         <v>30</v>
       </c>
-      <c r="F40" s="118">
+      <c r="F40" s="117">
         <v>2.4999999999999999E-7</v>
       </c>
       <c r="J40" t="s">
@@ -20305,7 +20280,7 @@
       <c r="E41">
         <v>575</v>
       </c>
-      <c r="F41" s="118">
+      <c r="F41" s="117">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J41" t="s">
@@ -20320,7 +20295,7 @@
       <c r="M41">
         <v>900</v>
       </c>
-      <c r="N41" s="118">
+      <c r="N41" s="117">
         <f>VLOOKUP("market for fibreboard, hard",Table3[],6,FALSE)+VLOOKUP("market for waste fibreboard",Table3[],6,FALSE)*Table1[[#This Row],[Density]]</f>
         <v>1.0900000000000001E-5</v>
       </c>
@@ -20341,7 +20316,7 @@
       <c r="E42">
         <v>1680</v>
       </c>
-      <c r="F42" s="118">
+      <c r="F42" s="117">
         <v>1E-10</v>
       </c>
       <c r="J42" t="s">
@@ -20356,7 +20331,7 @@
       <c r="M42">
         <v>700</v>
       </c>
-      <c r="N42" s="118">
+      <c r="N42" s="117">
         <f>VLOOKUP("market for fibreboard, soft",Table3[],6,FALSE)+VLOOKUP("market for waste fibreboard",Table3[],6,FALSE)*Table1[[#This Row],[Density]]</f>
         <v>3.2000000000000003E-6</v>
       </c>
@@ -20377,7 +20352,7 @@
       <c r="E43">
         <v>800</v>
       </c>
-      <c r="F43" s="118">
+      <c r="F43" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J43" t="s">
@@ -20416,7 +20391,7 @@
       <c r="E44">
         <v>700</v>
       </c>
-      <c r="F44" s="118">
+      <c r="F44" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J44" t="s">
@@ -20449,7 +20424,7 @@
       <c r="D45" t="s">
         <v>170</v>
       </c>
-      <c r="F45" s="118">
+      <c r="F45" s="117">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J45" t="s">
@@ -20485,8 +20460,7 @@
       <c r="D46" t="s">
         <v>170</v>
       </c>
-      <c r="E46" s="117"/>
-      <c r="F46" s="118">
+      <c r="F46" s="117">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J46" t="s">
@@ -20525,7 +20499,7 @@
       <c r="E47">
         <v>1100</v>
       </c>
-      <c r="F47" s="118">
+      <c r="F47" s="117">
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="J47" t="s">
@@ -20561,7 +20535,7 @@
       <c r="E48">
         <v>2160</v>
       </c>
-      <c r="F48" s="118">
+      <c r="F48" s="117">
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="J48" t="s">
@@ -20600,7 +20574,7 @@
       <c r="E49">
         <v>2300</v>
       </c>
-      <c r="F49" s="118">
+      <c r="F49" s="117">
         <v>7.5E-10</v>
       </c>
       <c r="J49" t="s">
@@ -20636,7 +20610,7 @@
       <c r="E50">
         <v>2800</v>
       </c>
-      <c r="F50" s="118">
+      <c r="F50" s="117">
         <v>2.5000000000000001E-9</v>
       </c>
       <c r="J50" t="s">
@@ -20672,7 +20646,7 @@
       <c r="E51">
         <v>750</v>
       </c>
-      <c r="F51" s="118">
+      <c r="F51" s="117">
         <v>2.5000000000000002E-6</v>
       </c>
       <c r="J51" t="s">
@@ -20705,7 +20679,7 @@
       <c r="D52" t="s">
         <v>46</v>
       </c>
-      <c r="F52" s="118">
+      <c r="F52" s="117">
         <v>2.4999999999999999E-7</v>
       </c>
       <c r="J52" t="s">
@@ -20738,7 +20712,7 @@
       <c r="D53" t="s">
         <v>46</v>
       </c>
-      <c r="F53" s="118">
+      <c r="F53" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="J53" t="s">
@@ -20777,7 +20751,7 @@
       <c r="E54">
         <v>560</v>
       </c>
-      <c r="F54" s="118">
+      <c r="F54" s="117">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J54" t="s">
@@ -20813,7 +20787,7 @@
       <c r="E55">
         <v>3.15</v>
       </c>
-      <c r="F55" s="118">
+      <c r="F55" s="117">
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J55" t="s">
@@ -20852,7 +20826,7 @@
       <c r="E56">
         <v>30</v>
       </c>
-      <c r="F56" s="118">
+      <c r="F56" s="117">
         <v>2.4999999999999999E-8</v>
       </c>
       <c r="J56" t="s">
@@ -20891,7 +20865,7 @@
       <c r="E57">
         <v>30</v>
       </c>
-      <c r="F57" s="118">
+      <c r="F57" s="117">
         <v>2.4999999999999999E-8</v>
       </c>
       <c r="J57" t="s">
@@ -20927,7 +20901,7 @@
       <c r="E58">
         <v>35</v>
       </c>
-      <c r="F58" s="118">
+      <c r="F58" s="117">
         <v>2.4999999999999999E-8</v>
       </c>
       <c r="J58" t="s">
@@ -20963,7 +20937,7 @@
       <c r="E59">
         <v>1350</v>
       </c>
-      <c r="F59" s="118">
+      <c r="F59" s="117">
         <v>1E-8</v>
       </c>
       <c r="J59" t="s">
@@ -21002,7 +20976,7 @@
       <c r="E60">
         <v>1920</v>
       </c>
-      <c r="F60" s="118">
+      <c r="F60" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J60" t="s">
@@ -21038,7 +21012,7 @@
       <c r="E61">
         <v>1845</v>
       </c>
-      <c r="F61" s="118">
+      <c r="F61" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J61" t="s">
@@ -21074,7 +21048,7 @@
       <c r="E62">
         <v>740</v>
       </c>
-      <c r="F62" s="118">
+      <c r="F62" s="117">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J62" t="s">
@@ -21110,7 +21084,7 @@
       <c r="E63">
         <v>500</v>
       </c>
-      <c r="F63" s="118">
+      <c r="F63" s="117">
         <v>7.5000000000000002E-6</v>
       </c>
       <c r="J63" t="s">
@@ -21143,7 +21117,7 @@
       <c r="D64" t="s">
         <v>38</v>
       </c>
-      <c r="F64" s="118">
+      <c r="F64" s="117">
         <v>9.9999999999999995E-8</v>
       </c>
       <c r="J64" t="s">
@@ -21182,7 +21156,7 @@
       <c r="E65">
         <v>2600</v>
       </c>
-      <c r="F65" s="118">
+      <c r="F65" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J65" t="s">
@@ -21218,7 +21192,7 @@
       <c r="E66">
         <v>1200</v>
       </c>
-      <c r="F66" s="118">
+      <c r="F66" s="117">
         <v>5.0000000000000001E-9</v>
       </c>
       <c r="J66" t="s">
@@ -21254,7 +21228,7 @@
       <c r="E67">
         <v>7800</v>
       </c>
-      <c r="F67" s="118">
+      <c r="F67" s="117">
         <v>7.4999999999999993E-9</v>
       </c>
       <c r="J67" t="s">
@@ -21290,7 +21264,7 @@
       <c r="E68">
         <v>20</v>
       </c>
-      <c r="F68" s="118">
+      <c r="F68" s="117">
         <v>7.4999999999999993E-9</v>
       </c>
       <c r="J68" t="s">
@@ -21323,7 +21297,7 @@
       <c r="D69" t="s">
         <v>38</v>
       </c>
-      <c r="F69" s="118">
+      <c r="F69" s="117">
         <v>1E-10</v>
       </c>
       <c r="J69" t="s">
@@ -21356,7 +21330,7 @@
       <c r="D70" t="s">
         <v>38</v>
       </c>
-      <c r="F70" s="118">
+      <c r="F70" s="117">
         <v>1E-10</v>
       </c>
       <c r="J70" t="s">
@@ -21386,7 +21360,7 @@
       <c r="D71" t="s">
         <v>38</v>
       </c>
-      <c r="F71" s="118">
+      <c r="F71" s="117">
         <v>5.0000000000000002E-11</v>
       </c>
       <c r="J71" t="s">
@@ -21416,7 +21390,7 @@
       <c r="D72" t="s">
         <v>38</v>
       </c>
-      <c r="F72" s="118">
+      <c r="F72" s="117">
         <v>9.9999999999999994E-12</v>
       </c>
       <c r="J72" t="s">
@@ -21446,7 +21420,7 @@
       <c r="D73" t="s">
         <v>38</v>
       </c>
-      <c r="F73" s="118">
+      <c r="F73" s="117">
         <v>1E-10</v>
       </c>
       <c r="J73" t="s">
@@ -21479,7 +21453,7 @@
       <c r="D74" t="s">
         <v>38</v>
       </c>
-      <c r="F74" s="118">
+      <c r="F74" s="117">
         <v>1E-10</v>
       </c>
       <c r="J74" t="s">
@@ -21512,7 +21486,7 @@
       <c r="D75" t="s">
         <v>38</v>
       </c>
-      <c r="F75" s="118">
+      <c r="F75" s="117">
         <v>1E-10</v>
       </c>
     </row>
@@ -21529,7 +21503,7 @@
       <c r="D76" t="s">
         <v>38</v>
       </c>
-      <c r="F76" s="118">
+      <c r="F76" s="117">
         <v>5.0000000000000002E-11</v>
       </c>
     </row>
@@ -21546,7 +21520,7 @@
       <c r="D77" t="s">
         <v>38</v>
       </c>
-      <c r="F77" s="118">
+      <c r="F77" s="117">
         <v>5.0000000000000002E-11</v>
       </c>
     </row>
@@ -21563,7 +21537,7 @@
       <c r="D78" t="s">
         <v>38</v>
       </c>
-      <c r="F78" s="118">
+      <c r="F78" s="117">
         <v>1E-10</v>
       </c>
       <c r="J78" t="s">
@@ -21583,7 +21557,7 @@
       <c r="D79" t="s">
         <v>38</v>
       </c>
-      <c r="F79" s="118">
+      <c r="F79" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J79" t="s">
@@ -21603,7 +21577,7 @@
       <c r="D80" t="s">
         <v>38</v>
       </c>
-      <c r="F80" s="118">
+      <c r="F80" s="117">
         <v>1E-10</v>
       </c>
       <c r="J80" t="s">
@@ -21623,7 +21597,7 @@
       <c r="D81" t="s">
         <v>38</v>
       </c>
-      <c r="F81" s="118">
+      <c r="F81" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
       <c r="J81" t="s">
@@ -21643,7 +21617,7 @@
       <c r="D82" t="s">
         <v>38</v>
       </c>
-      <c r="F82" s="118">
+      <c r="F82" s="117">
         <v>5.0000000000000002E-11</v>
       </c>
     </row>
@@ -21660,7 +21634,7 @@
       <c r="D83" t="s">
         <v>38</v>
       </c>
-      <c r="F83" s="118">
+      <c r="F83" s="117">
         <v>5.0000000000000002E-11</v>
       </c>
     </row>
@@ -21677,7 +21651,7 @@
       <c r="D84" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="118">
+      <c r="F84" s="117">
         <v>5.0000000000000001E-9</v>
       </c>
     </row>
@@ -21694,7 +21668,7 @@
       <c r="D85" t="s">
         <v>38</v>
       </c>
-      <c r="F85" s="118">
+      <c r="F85" s="117">
         <v>1E-10</v>
       </c>
     </row>
@@ -21711,7 +21685,7 @@
       <c r="D86" t="s">
         <v>38</v>
       </c>
-      <c r="F86" s="118">
+      <c r="F86" s="117">
         <v>1E-8</v>
       </c>
     </row>
@@ -21728,7 +21702,7 @@
       <c r="D87" t="s">
         <v>38</v>
       </c>
-      <c r="F87" s="118">
+      <c r="F87" s="117">
         <v>1E-8</v>
       </c>
     </row>
@@ -21745,7 +21719,7 @@
       <c r="D88" t="s">
         <v>38</v>
       </c>
-      <c r="F88" s="118">
+      <c r="F88" s="117">
         <v>5.0000000000000001E-9</v>
       </c>
     </row>
@@ -21762,7 +21736,7 @@
       <c r="D89" t="s">
         <v>38</v>
       </c>
-      <c r="F89" s="118">
+      <c r="F89" s="117">
         <v>5.0000000000000001E-9</v>
       </c>
     </row>
@@ -21779,7 +21753,7 @@
       <c r="D90" t="s">
         <v>38</v>
       </c>
-      <c r="F90" s="118">
+      <c r="F90" s="117">
         <v>5.0000000000000003E-10</v>
       </c>
     </row>
@@ -21796,7 +21770,7 @@
       <c r="D91" t="s">
         <v>46</v>
       </c>
-      <c r="F91" s="118">
+      <c r="F91" s="117">
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
@@ -21813,7 +21787,7 @@
       <c r="D92" t="s">
         <v>46</v>
       </c>
-      <c r="F92" s="118">
+      <c r="F92" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
@@ -21830,7 +21804,7 @@
       <c r="D93" t="s">
         <v>46</v>
       </c>
-      <c r="F93" s="118">
+      <c r="F93" s="117">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
@@ -21847,7 +21821,7 @@
       <c r="D94" t="s">
         <v>46</v>
       </c>
-      <c r="F94" s="118">
+      <c r="F94" s="117">
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
@@ -21867,7 +21841,7 @@
       <c r="E95">
         <v>65</v>
       </c>
-      <c r="F95" s="118">
+      <c r="F95" s="117">
         <v>1E-8</v>
       </c>
     </row>
@@ -21887,7 +21861,7 @@
       <c r="E96">
         <v>7140</v>
       </c>
-      <c r="F96" s="118">
+      <c r="F96" s="117">
         <v>1E-8</v>
       </c>
     </row>
@@ -21904,7 +21878,7 @@
       <c r="D97" t="s">
         <v>198</v>
       </c>
-      <c r="F97" s="118">
+      <c r="F97" s="117">
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
@@ -21921,7 +21895,7 @@
       <c r="D98" t="s">
         <v>275</v>
       </c>
-      <c r="F98" s="118">
+      <c r="F98" s="117">
         <v>5.0000000000000003E-10</v>
       </c>
     </row>
@@ -21938,7 +21912,7 @@
       <c r="D99" t="s">
         <v>38</v>
       </c>
-      <c r="F99" s="118">
+      <c r="F99" s="117">
         <v>5.0000000000000002E-11</v>
       </c>
     </row>
@@ -21955,7 +21929,7 @@
       <c r="D100" t="s">
         <v>46</v>
       </c>
-      <c r="F100" s="118">
+      <c r="F100" s="117">
         <v>1E-8</v>
       </c>
     </row>
@@ -21972,7 +21946,7 @@
       <c r="D101" t="s">
         <v>46</v>
       </c>
-      <c r="F101" s="118">
+      <c r="F101" s="117">
         <v>1E-8</v>
       </c>
     </row>
@@ -21989,7 +21963,7 @@
       <c r="D102" t="s">
         <v>46</v>
       </c>
-      <c r="F102" s="118">
+      <c r="F102" s="117">
         <v>1E-8</v>
       </c>
     </row>
@@ -22006,7 +21980,7 @@
       <c r="D103" t="s">
         <v>46</v>
       </c>
-      <c r="F103" s="118">
+      <c r="F103" s="117">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
@@ -22023,7 +21997,7 @@
       <c r="D104" t="s">
         <v>46</v>
       </c>
-      <c r="F104" s="118">
+      <c r="F104" s="117">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
@@ -22040,7 +22014,7 @@
       <c r="D105" t="s">
         <v>46</v>
       </c>
-      <c r="F105" s="118">
+      <c r="F105" s="117">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
@@ -22057,7 +22031,7 @@
       <c r="D106" t="s">
         <v>38</v>
       </c>
-      <c r="F106" s="118">
+      <c r="F106" s="117">
         <v>1E-10</v>
       </c>
     </row>
@@ -22074,7 +22048,7 @@
       <c r="D107" t="s">
         <v>38</v>
       </c>
-      <c r="F107" s="118">
+      <c r="F107" s="117">
         <v>1E-10</v>
       </c>
     </row>
@@ -22094,7 +22068,7 @@
       <c r="E108">
         <v>7140</v>
       </c>
-      <c r="F108" s="118">
+      <c r="F108" s="117">
         <v>1E-10</v>
       </c>
     </row>
@@ -22125,6 +22099,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="132423e5-a7cd-4a14-95a1-f4cfc4bc40a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fdfa86f3-4908-469f-b054-c40076a06775" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E38A60D41FCFC45940D6B62EA5A5EF9" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ae232b6878c9823338cde463659ceee5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="132423e5-a7cd-4a14-95a1-f4cfc4bc40a3" xmlns:ns3="fdfa86f3-4908-469f-b054-c40076a06775" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cacca41beb2bb026b555beeb3907f258" ns2:_="" ns3:_="">
     <xsd:import namespace="132423e5-a7cd-4a14-95a1-f4cfc4bc40a3"/>
@@ -22335,27 +22329,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{784B5EF4-25DE-4AB6-943C-95908AD54A26}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fdfa86f3-4908-469f-b054-c40076a06775"/>
+    <ds:schemaRef ds:uri="132423e5-a7cd-4a14-95a1-f4cfc4bc40a3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="132423e5-a7cd-4a14-95a1-f4cfc4bc40a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fdfa86f3-4908-469f-b054-c40076a06775" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CDEB65-86A0-4320-8434-0830F2C39515}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5DF09E0-BB4F-45B4-AE8A-9FCA5AC1BE58}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22372,29 +22371,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CDEB65-86A0-4320-8434-0830F2C39515}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{784B5EF4-25DE-4AB6-943C-95908AD54A26}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fdfa86f3-4908-469f-b054-c40076a06775"/>
-    <ds:schemaRef ds:uri="132423e5-a7cd-4a14-95a1-f4cfc4bc40a3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>